<commit_message>
CS IA /RetroTrack/ SC5 (final draft) 4/27/2025
</commit_message>
<xml_diff>
--- a/uploads/Delivery_Data_test.xlsx
+++ b/uploads/Delivery_Data_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90311852-9224-4796-B105-04C87E1C1D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0512A3EB-AE03-4D80-B501-035078B4F0F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19406" windowHeight="12206" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="78">
   <si>
     <t>Base Address</t>
   </si>
@@ -50,69 +50,9 @@
     <t>Expected Delivery Cost (VND)</t>
   </si>
   <si>
-    <t>12 Đông Hưng Thuận 10, KP.3, P. Đông Hưng Thuận, Quận 12, TP. HCM</t>
-  </si>
-  <si>
-    <t>100 Lý Thường Kiệt, Phường 6, Cà Mau</t>
-  </si>
-  <si>
-    <t>30 Đinh Tiên Hoàng, Thành phố Ninh Bình, Ninh Bình</t>
-  </si>
-  <si>
-    <t>34 Ba Cu, Phường 1, Vũng Tàu</t>
-  </si>
-  <si>
-    <t>03 Nguyễn Chí Thanh, Phường 1, Đà Lạt</t>
-  </si>
-  <si>
-    <t>250 Nguyễn Văn Linh, Hải Châu, Đà Nẵng</t>
-  </si>
-  <si>
     <t>90 Lê Thánh Tông, Thành phố Buôn Ma Thuột, Đắk Lắk</t>
   </si>
   <si>
-    <t>98 Trần Đăng Ninh, Thành phố Lạng Sơn, Lạng Sơn</t>
-  </si>
-  <si>
-    <t>25 Mậu Thân, Ninh Kiều, Cần Thơ</t>
-  </si>
-  <si>
-    <t>20 Nguyễn Lương Bằng, Thành phố Hải Dương, Hải Dương</t>
-  </si>
-  <si>
-    <t>40 Phan Đình Phùng, Thành phố Pleiku, Gia Lai</t>
-  </si>
-  <si>
-    <t>12 Lê Lợi, Thành phố Huế, Thừa Thiên Huế</t>
-  </si>
-  <si>
-    <t>45 Trần Hưng Đạo, Thành phố Nam Định, Nam Định</t>
-  </si>
-  <si>
-    <t>Số 1 Hoàng Đạo Thúy, Thanh Xuân, Hà Nội</t>
-  </si>
-  <si>
-    <t>88 Nguyễn Trãi, Thành phố Thanh Hóa, Thanh Hóa</t>
-  </si>
-  <si>
-    <t>20 Trần Phú, Phường 3, Bạc Liêu</t>
-  </si>
-  <si>
-    <t>120 Nguyễn Tất Thành, Thành phố Quy Nhơn, Bình Định</t>
-  </si>
-  <si>
-    <t>70 Lý Thường Kiệt, Thành phố Bắc Giang, Bắc Giang</t>
-  </si>
-  <si>
-    <t>56 Trần Phú, Nha Trang, Khánh Hòa</t>
-  </si>
-  <si>
-    <t>55 Trần Phú, Thành phố Hà Giang, Hà Giang</t>
-  </si>
-  <si>
-    <t>15 Lạch Tray, Quận Ngô Quyền, Hải Phòng</t>
-  </si>
-  <si>
     <t>Shipping Address</t>
   </si>
   <si>
@@ -120,6 +60,213 @@
   </si>
   <si>
     <t>Actual Delivery Cost (VND)</t>
+  </si>
+  <si>
+    <t>1 Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng</t>
+  </si>
+  <si>
+    <t>98 Trần Đăng Ninh, Hoàng Văn Thụ, Thành phố Lạng Sơn, Lạng Sơn</t>
+  </si>
+  <si>
+    <t>129, Lý Thường Kiệt, Phường 6, Cà Mau, Cà Mau Province, Vietnam</t>
+  </si>
+  <si>
+    <t>Ninh Bình, Ninh Binh, Vietnam</t>
+  </si>
+  <si>
+    <t>31A, Ba Cu, Ward 1, Vũng Tàu, Ba Ria-Vung Tau 797979, Vietnam</t>
+  </si>
+  <si>
+    <t>07, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lam Dong 02633, Vietnam</t>
+  </si>
+  <si>
+    <t>184, Đường Nguyễn Văn Linh, Thanh Khê District, Đà Nẵng, 50207, Vietnam</t>
+  </si>
+  <si>
+    <t>Buon Ma Thuot, Dak Lak, Vietnam</t>
+  </si>
+  <si>
+    <t>10, Đông Hưng Thuận 10, District 12, Ho Chi Minh City, 71507, Vietnam</t>
+  </si>
+  <si>
+    <t>25A, Đường Mậu Thân, Ninh Kiều District, Cần Thơ, 94108, Vietnam</t>
+  </si>
+  <si>
+    <t>20, Nguyễn Lương Bằng, Lương Bằng, Hưng Yên Province, Vietnam</t>
+  </si>
+  <si>
+    <t>40, Phan Đình Phùng, Pleiku, Gia Lai Province 61111, Vietnam</t>
+  </si>
+  <si>
+    <t>Quoc Hoc Hue High School for the Gifted, 12, Lê Lợi, Thuận Hóa District, Huế, 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>45, Trần Hưng Đạo, Nam Định, Nam Định Province 42000, Vietnam</t>
+  </si>
+  <si>
+    <t>24T1, 1 Hoàng Đạo Thúy, Hanoi, Ha Noi 10055, Vietnam</t>
+  </si>
+  <si>
+    <t>Thanh Hóa, Thanh Hoa, Vietnam</t>
+  </si>
+  <si>
+    <t>3, Ba Cu, Vũng Tàu, Ba Ria-Vung Tau 78207, Vietnam</t>
+  </si>
+  <si>
+    <t>20, Trần Phú, Phường 3, Bạc Liêu, Bạc Liêu Province 97000, Vietnam</t>
+  </si>
+  <si>
+    <t>Trung tâm Hội nghị tỉnh Bình Định, 1, Nguyễn Tất Thành, Phường Trần Phú, Quy Nhơn, Bình Định Province 55106, Vietnam</t>
+  </si>
+  <si>
+    <t>25, Nguyễn Lương Bằng, Lương Bằng, Hưng Yên Province, Vietnam</t>
+  </si>
+  <si>
+    <t>Ngõ 20 Đường Đình Hương, Phường Đông Cương, Thanh Hóa, Thanh Hóa Province 45000, Vietnam</t>
+  </si>
+  <si>
+    <t>120, Nguyễn Tất Thành, Phường Trần Phú, Quy Nhơn, Bình Định Province 55106, Vietnam</t>
+  </si>
+  <si>
+    <t>70, Lý Thường Kiệt, Thắng, Bắc Giang Province, Vietnam</t>
+  </si>
+  <si>
+    <t>03, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng Province 02633, Vietnam</t>
+  </si>
+  <si>
+    <t>Phong Lan Guesthouse, 12/66, Lê Lợi, Thuận Hóa District, Huế, 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>Lý Thường Kiệt, Phường 7, Cà Mau, Cà Mau Province, Vietnam</t>
+  </si>
+  <si>
+    <t>Len's Cafe, 07, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng Province 02633, Vietnam</t>
+  </si>
+  <si>
+    <t>Nhà 24T2 KĐT Trung Hoà Nhân Chính - Hoàng Đạo Thúy, Phố Hoàng Đạo Thúy, Cầu Giấy District, Hà Nội, 10055, Vietnam</t>
+  </si>
+  <si>
+    <t>11, Kiệt 11, Thuận Hóa District, Huế, 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>10, Trần Hưng Đạo, Tam Điệp, Ninh Bình Province, Vietnam</t>
+  </si>
+  <si>
+    <t>16, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lam Dong 02633, Vietnam</t>
+  </si>
+  <si>
+    <t>250, Đường Nguyễn Văn Linh, Thanh Khê District, Đà Nẵng, 50207, Vietnam</t>
+  </si>
+  <si>
+    <t>56, Tran Phu, Vĩnh Nguyên, Nha Trang, Khánh Hòa Province 57131, Vietnam</t>
+  </si>
+  <si>
+    <t>454, Trần Hưng Đạo, Nam Định, Nam Định Province 42000, Vietnam</t>
+  </si>
+  <si>
+    <t>28, Lý Thường Kiệt, Phường 6, Cà Mau, Cà Mau Province, Vietnam</t>
+  </si>
+  <si>
+    <t>173/24/7, Hoàng Hoa Thám, Ba Đình District, Hà Nội, 10000, Vietnam</t>
+  </si>
+  <si>
+    <t>47, Phan Đình Phùng, Pleiku, Gia Lai Province 61111, Vietnam</t>
+  </si>
+  <si>
+    <t>Đại học Duy Tân, 254, Đường Nguyễn Văn Linh, Thanh Khê District, Đà Nẵng, 50207, Vietnam</t>
+  </si>
+  <si>
+    <t>289, Trần Hưng Đạo, Nam Định, Nam Định Province 42000, Vietnam</t>
+  </si>
+  <si>
+    <t>123, Lê Lợi, Thuận Hóa District, Huế, 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>25A, Đường Mậu Thân, Ninha Kiều District, Cần Thơ, 94108, Vietnam</t>
+  </si>
+  <si>
+    <t>55, Tran Phu Street, Trần Phú, Hà Giang, Hà Giang Province 20152, Vietnam</t>
+  </si>
+  <si>
+    <t>10, Trần Hưng Đạo, Nam Định, Nam Định Province 42000, Vietnam</t>
+  </si>
+  <si>
+    <t>98, Trần Đăng Ninh, Mường Thanh, Điện Biên Phủ, Điện Biên Province 32000, Vietnam</t>
+  </si>
+  <si>
+    <t>98, National Route 12, Mường Thanh, Điện Biên Phủ, Điện Biên Province 32000, Vietnam</t>
+  </si>
+  <si>
+    <t>33, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng Province 02633, Vietnam</t>
+  </si>
+  <si>
+    <t>Thanh Hóa, Quốc lộ 15, Hồi Xuân, Thanh Hóa Province, Vietnam</t>
+  </si>
+  <si>
+    <t>34-36, Đường Tôn Đức Thắng, Bắc Giang, Bắc Giang Province 26000, Vietnam</t>
+  </si>
+  <si>
+    <t>20, Nguyễn Lương Bằng, Phường Thanh Bình, Hải Dương, Hải Dương Province 03118, Vietnam</t>
+  </si>
+  <si>
+    <t>144, Đường Nguyễn Văn Linh, Hải Châu District, Đà Nẵng, 50207, Vietnam</t>
+  </si>
+  <si>
+    <t>Thuy Hoa Spa, 71, Minh Khai Road, Phường Tương Giang, Từ Sơn, Bắc Ninh Province 16300, Vietnam</t>
+  </si>
+  <si>
+    <t>100, Lý Thường Kiệt, Phường 7, Cà Mau, Cà Mau Province, Vietnam</t>
+  </si>
+  <si>
+    <t>12, Lê Lợi, Thuận Hóa District, Huế, Thura Thien-Hue 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>Bong hostel, 55, Nguyen Thai Hoc Street, Minh Khai, Hà Giang, Hà Giang Province 20152, Vietnam</t>
+  </si>
+  <si>
+    <t>Ngô Quyền District, Hải Phòng, Vietnam</t>
+  </si>
+  <si>
+    <t>Hanoi, 120, Le Duan Road, Hoàn Kiếm District, Hà Nội, 11018, Vietnam</t>
+  </si>
+  <si>
+    <t>Hoa Lư, Ninh Bình Province, Vietnam</t>
+  </si>
+  <si>
+    <t>Khánh Huyền Smartphone, 178, Đường Ngô Quyền, Hải Phòng, 35999, Vietnam</t>
+  </si>
+  <si>
+    <t>20, Nguyễn Lương Bằng, Phường Tứ Minh, Hải Dương, Hải Dương Province 03118, Vietnam</t>
+  </si>
+  <si>
+    <t>70, Đường Tôn Đức Thắng 1, Bắc Giang, Bắc Giang Province 26000, Vietnam</t>
+  </si>
+  <si>
+    <t>56, Tran Phu, Lộc Thọ, Nha Trang, Khánh Hòa Province 48058, Vietnam</t>
+  </si>
+  <si>
+    <t>Quán Nhí, 16, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng Province 66113, Vietnam</t>
+  </si>
+  <si>
+    <t>12/66, Lê Lợi, Huế, Thura Thien-Hue 54000, Vietnam</t>
+  </si>
+  <si>
+    <t>Đắk Lắk Province, Vietnam</t>
+  </si>
+  <si>
+    <t>Petrolimex 888, Đường Nguyễn Trãi, Phường Trúc Lâm, Nghi Sơn, Thanh Hoa province, Vietnam</t>
+  </si>
+  <si>
+    <t>Da Nang, Vietnam</t>
+  </si>
+  <si>
+    <t>UBND Thành phố Ninh Bình, Đường Lê Đại Hành, Hoa Lư, Ninh Binh province 08000, Vietnam</t>
+  </si>
+  <si>
+    <t>Thanh Hóa, Thanh Hóa Province, Vietnam</t>
+  </si>
+  <si>
+    <t>03, Nguyễn Chí Thanh, Phường 1, Đà Lạt, Lâm Đồng Province 66113, Vietnam</t>
   </si>
 </sst>
 </file>
@@ -215,10 +362,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,14 +653,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="70.765625" customWidth="1"/>
-    <col min="2" max="2" width="59.921875" customWidth="1"/>
+    <col min="2" max="2" width="108.23046875" customWidth="1"/>
     <col min="3" max="3" width="42.921875" customWidth="1"/>
     <col min="4" max="4" width="28.69140625" customWidth="1"/>
     <col min="5" max="5" width="28.4609375" customWidth="1"/>
@@ -531,7 +674,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -546,18 +689,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -576,10 +719,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4">
         <v>45605</v>
@@ -604,10 +747,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>45605</v>
@@ -630,10 +773,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4">
         <v>45605</v>
@@ -658,10 +801,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>45607</v>
@@ -686,10 +829,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C7" s="4">
         <v>45608</v>
@@ -714,10 +857,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="4">
         <v>45608</v>
@@ -742,7 +885,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -770,10 +913,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C10" s="4">
         <v>45608</v>
@@ -798,10 +941,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4">
         <v>45609</v>
@@ -826,10 +969,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4">
         <v>45609</v>
@@ -854,10 +997,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4">
         <v>45609</v>
@@ -882,10 +1025,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4">
         <v>45609</v>
@@ -910,10 +1053,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C15" s="4">
         <v>45610</v>
@@ -938,10 +1081,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4">
         <v>45610</v>
@@ -966,10 +1109,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C17" s="4">
         <v>45610</v>
@@ -994,10 +1137,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4">
         <v>45610</v>
@@ -1022,10 +1165,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C19" s="4">
         <v>45611</v>
@@ -1050,10 +1193,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C20" s="4">
         <v>45611</v>
@@ -1078,10 +1221,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C21" s="4">
         <v>45611</v>
@@ -1106,10 +1249,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C22" s="4">
         <v>45611</v>
@@ -1134,10 +1277,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4">
         <v>45611</v>
@@ -1162,10 +1305,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C24" s="4">
         <v>45604</v>
@@ -1190,10 +1333,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4">
         <v>45605</v>
@@ -1218,10 +1361,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C26" s="4">
         <v>45607</v>
@@ -1246,10 +1389,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C27" s="4">
         <v>45608</v>
@@ -1274,10 +1417,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C28" s="4">
         <v>45609</v>
@@ -1302,10 +1445,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C29" s="4">
         <v>45608</v>
@@ -1330,10 +1473,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C30" s="4">
         <v>45607</v>
@@ -1358,10 +1501,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C31" s="4">
         <v>45616</v>
@@ -1386,10 +1529,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C32" s="4">
         <v>45616</v>
@@ -1414,10 +1557,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="C33" s="4">
         <v>45616</v>
@@ -1442,10 +1585,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="C34" s="4">
         <v>45616</v>
@@ -1470,10 +1613,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C35" s="4">
         <v>45615</v>
@@ -1498,10 +1641,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="C36" s="4">
         <v>45614</v>
@@ -1526,10 +1669,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C37" s="4">
         <v>45612</v>
@@ -1554,10 +1697,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C38" s="4">
         <v>45617</v>
@@ -1582,10 +1725,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C39" s="4">
         <v>45616</v>
@@ -1610,10 +1753,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C40" s="4">
         <v>45617</v>
@@ -1638,10 +1781,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C41" s="4">
         <v>45602</v>
@@ -1666,10 +1809,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C42" s="4">
         <v>45604</v>
@@ -1694,10 +1837,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C43" s="4">
         <v>45604</v>
@@ -1722,10 +1865,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C44" s="4">
         <v>45604</v>
@@ -1750,10 +1893,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C45" s="4">
         <v>45605</v>
@@ -1778,10 +1921,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C46" s="4">
         <v>45605</v>
@@ -1806,10 +1949,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C47" s="4">
         <v>45609</v>
@@ -1834,10 +1977,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C48" s="4">
         <v>45610</v>
@@ -1862,10 +2005,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="C49" s="4">
         <v>45610</v>
@@ -1890,10 +2033,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C50" s="4">
         <v>45610</v>
@@ -1918,10 +2061,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C51" s="4">
         <v>45610</v>
@@ -1946,10 +2089,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C52" s="4">
         <v>45614</v>
@@ -1974,10 +2117,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C53" s="4">
         <v>45614</v>
@@ -2002,10 +2145,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="C54" s="4">
         <v>45614</v>
@@ -2030,10 +2173,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C55" s="4">
         <v>45618</v>
@@ -2058,10 +2201,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="C56" s="4">
         <v>45618</v>
@@ -2086,10 +2229,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C57" s="4">
         <v>45618</v>
@@ -2114,10 +2257,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C58" s="4">
         <v>45614</v>
@@ -2142,10 +2285,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C59" s="4">
         <v>45612</v>
@@ -2170,10 +2313,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C60" s="4">
         <v>45617</v>
@@ -2198,10 +2341,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C61" s="4">
         <v>45621</v>
@@ -2226,10 +2369,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="C62" s="4">
         <v>45621</v>
@@ -2254,10 +2397,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A63" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C63" s="4">
         <v>45621</v>
@@ -2282,10 +2425,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C64" s="4">
         <v>45621</v>
@@ -2310,10 +2453,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C65" s="4">
         <v>45621</v>
@@ -2338,10 +2481,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C66" s="4">
         <v>45617</v>
@@ -2366,10 +2509,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C67" s="4">
         <v>45619</v>
@@ -2394,10 +2537,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="C68" s="4">
         <v>45619</v>
@@ -2422,10 +2565,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C69" s="4">
         <v>45615</v>
@@ -2450,10 +2593,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C70" s="4">
         <v>45618</v>
@@ -2478,10 +2621,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C71" s="4">
         <v>45612</v>
@@ -2506,10 +2649,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C72" s="4">
         <v>45621</v>
@@ -2534,10 +2677,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C73" s="4">
         <v>45621</v>
@@ -2562,10 +2705,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C74" s="4">
         <v>45621</v>
@@ -2590,10 +2733,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C75" s="4">
         <v>45621</v>
@@ -2618,10 +2761,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C76" s="4">
         <v>45615</v>
@@ -2646,10 +2789,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="C77" s="4">
         <v>45615</v>
@@ -2674,10 +2817,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C78" s="4">
         <v>45614</v>
@@ -2702,10 +2845,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C79" s="4">
         <v>45614</v>
@@ -2730,10 +2873,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A80" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="C80" s="4">
         <v>45614</v>
@@ -2758,10 +2901,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C81" s="4">
         <v>45614</v>
@@ -2786,10 +2929,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C82" s="4">
         <v>45615</v>
@@ -2814,10 +2957,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="C83" s="4">
         <v>45615</v>
@@ -2842,10 +2985,10 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C84" s="4">
         <v>45617</v>
@@ -2870,10 +3013,10 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="C85" s="4">
         <v>45617</v>
@@ -2898,10 +3041,10 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A86" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C86" s="4">
         <v>45617</v>
@@ -2926,10 +3069,10 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A87" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C87" s="4">
         <v>45618</v>
@@ -2954,10 +3097,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A88" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C88" s="4">
         <v>45618</v>
@@ -2982,10 +3125,10 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C89" s="4">
         <v>45618</v>
@@ -3010,10 +3153,10 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C90" s="4">
         <v>45618</v>
@@ -3038,10 +3181,10 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C91" s="4">
         <v>45618</v>
@@ -3066,10 +3209,10 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C92" s="4">
         <v>45618</v>
@@ -3094,10 +3237,10 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C93" s="4">
         <v>45618</v>
@@ -3122,10 +3265,10 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C94" s="4">
         <v>45618</v>
@@ -3150,10 +3293,10 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A95" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C95" s="4">
         <v>45609</v>
@@ -3178,10 +3321,10 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C96" s="4">
         <v>45609</v>
@@ -3206,10 +3349,10 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A97" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C97" s="4">
         <v>45616</v>
@@ -3234,10 +3377,10 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A98" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C98" s="4">
         <v>45616</v>
@@ -3253,7 +3396,7 @@
         <v>1397647.0588235296</v>
       </c>
       <c r="G98" s="3">
-        <f t="shared" ref="G98:G129" si="7" xml:space="preserve"> H98*E98</f>
+        <f t="shared" ref="G98:G123" si="7" xml:space="preserve"> H98*E98</f>
         <v>254117.64705882355</v>
       </c>
       <c r="H98" s="3">
@@ -3262,10 +3405,10 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="C99" s="4">
         <v>45616</v>
@@ -3290,10 +3433,10 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A100" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C100" s="4">
         <v>45319</v>
@@ -3318,10 +3461,10 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A101" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C101" s="4">
         <v>45623</v>
@@ -3346,10 +3489,10 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A102" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C102" s="4">
         <v>45623</v>
@@ -3374,10 +3517,10 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A103" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>19</v>
+        <v>73</v>
       </c>
       <c r="C103" s="4">
         <v>45622</v>
@@ -3402,10 +3545,10 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A104" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C104" s="4">
         <v>45624</v>
@@ -3430,10 +3573,10 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A105" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C105" s="4">
         <v>45624</v>
@@ -3458,10 +3601,10 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A106" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="C106" s="4">
         <v>45619</v>
@@ -3486,10 +3629,10 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A107" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C107" s="4">
         <v>45624</v>
@@ -3514,10 +3657,10 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A108" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C108" s="4">
         <v>45623</v>
@@ -3542,10 +3685,10 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A109" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C109" s="4">
         <v>45624</v>
@@ -3570,10 +3713,10 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A110" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="C110" s="4">
         <v>45624</v>
@@ -3598,10 +3741,10 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A111" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="C111" s="4">
         <v>45625</v>
@@ -3626,10 +3769,10 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A112" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C112" s="4">
         <v>45615</v>
@@ -3654,10 +3797,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A113" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C113" s="4">
         <v>45615</v>
@@ -3682,10 +3825,10 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A114" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="C114" s="4">
         <v>45618</v>
@@ -3710,10 +3853,10 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A115" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C115" s="4">
         <v>45618</v>
@@ -3738,10 +3881,10 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A116" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C116" s="4">
         <v>45618</v>
@@ -3766,10 +3909,10 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A117" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C117" s="4">
         <v>45610</v>
@@ -3794,10 +3937,10 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A118" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C118" s="4">
         <v>45610</v>
@@ -3822,10 +3965,10 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A119" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="C119" s="4">
         <v>45614</v>
@@ -3850,10 +3993,10 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A120" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="C120" s="4">
         <v>45619</v>
@@ -3878,10 +4021,10 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A121" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="C121" s="4">
         <v>45624</v>
@@ -3906,10 +4049,10 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A122" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C122" s="4">
         <v>45625</v>
@@ -3934,10 +4077,10 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A123" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C123" s="4">
         <v>45625</v>
@@ -3962,10 +4105,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bf3fe663-f7f5-4027-a36a-d4a2330d5d87" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CAA30FF95DE9534399CE3B501231BB74" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3c4f0e72d71b8778f6593c5c5d9e79ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bf3fe663-f7f5-4027-a36a-d4a2330d5d87" xmlns:ns4="e874b832-050d-4104-b40b-f84fdd73f121" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="17c92ad5ea96452abf2e06da8602a4f9" ns3:_="" ns4:_="">
     <xsd:import namespace="bf3fe663-f7f5-4027-a36a-d4a2330d5d87"/>
@@ -4204,24 +4365,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD17E36-EACE-4793-A28E-3BD0797FAB61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bf3fe663-f7f5-4027-a36a-d4a2330d5d87" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5897A43A-FD74-4F82-B631-A3EEDFA799B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e874b832-050d-4104-b40b-f84fdd73f121"/>
+    <ds:schemaRef ds:uri="bf3fe663-f7f5-4027-a36a-d4a2330d5d87"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C259E27C-6745-4B4E-9B29-FE0E6B7E78AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4238,29 +4407,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD17E36-EACE-4793-A28E-3BD0797FAB61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5897A43A-FD74-4F82-B631-A3EEDFA799B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e874b832-050d-4104-b40b-f84fdd73f121"/>
-    <ds:schemaRef ds:uri="bf3fe663-f7f5-4027-a36a-d4a2330d5d87"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>